<commit_message>
printing accuracies for random forest
</commit_message>
<xml_diff>
--- a/figures/confusion matrices_updated_20221207.xlsx
+++ b/figures/confusion matrices_updated_20221207.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
   <si>
     <t xml:space="preserve">SF2 BCells </t>
   </si>
@@ -97,28 +97,82 @@
     <t xml:space="preserve">Actual                 </t>
   </si>
   <si>
+    <t xml:space="preserve">Fig 5 F</t>
+  </si>
+  <si>
     <t xml:space="preserve">CD69+        141     13</t>
   </si>
   <si>
+    <t xml:space="preserve">SF7 B</t>
+  </si>
+  <si>
     <t xml:space="preserve">CD69-         11    198</t>
   </si>
   <si>
     <t xml:space="preserve">logistic regression</t>
   </si>
   <si>
-    <t xml:space="preserve">Fig 5 F</t>
+    <t xml:space="preserve">--- F4 D Accuracies --- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F2 D : B Cell Accuracies - Random Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SF 5 B : all cell activation accuracies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'NADH features': 0.9155313351498637,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'all features': 0.9274563820018366,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'all feautres': 0.9274563820018366,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'all features': 0.9264305177111717,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'nadh_features': 0.9054178145087236,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'nadh features': 0.9054178145087236,</t>
   </si>
   <si>
     <t xml:space="preserve">CD69+        140     14</t>
   </si>
   <si>
-    <t xml:space="preserve">SF7 B</t>
+    <t xml:space="preserve"> 'top 1': 0.6158038147138964,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'redox': 0.6657483930211203,</t>
   </si>
   <si>
     <t xml:space="preserve">CD69-         12    197</t>
   </si>
   <si>
+    <t xml:space="preserve"> 'top 2': 0.8119891008174387,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'top_1': 0.6951331496786042,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'top 3': 0.8937329700272479,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'top_2': 0.8617998163452709,</t>
+  </si>
+  <si>
     <t>SVM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'top 4': 0.9237057220708447}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'top_3': 0.8907254361799817,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'top_4': 0.9067952249770431}</t>
   </si>
   <si>
     <t xml:space="preserve">CD69+        138     16</t>
@@ -989,7 +1043,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="100" workbookViewId="0">
       <selection activeCell="R22" activeCellId="0" sqref="R22"/>
     </sheetView>
   </sheetViews>
@@ -1095,19 +1149,67 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4">
+        <v>0.9173553719008265</v>
+      </c>
+      <c r="I4">
+        <v>0.60835629017447201</v>
+      </c>
+      <c r="J4">
+        <v>0.80991735537190079</v>
+      </c>
+      <c r="K4">
+        <v>0.86225895316804413</v>
+      </c>
+      <c r="L4">
+        <v>0.88705234159779611</v>
+      </c>
+      <c r="M4">
+        <v>0.87235996326905418</v>
+      </c>
+      <c r="N4">
+        <v>0.37741046831955921</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5">
+        <v>0.99068100358422939</v>
+      </c>
+      <c r="I5">
+        <v>0.87813620071684584</v>
+      </c>
+      <c r="J5">
+        <v>0.95483870967741935</v>
+      </c>
+      <c r="K5">
+        <v>0.97347670250896057</v>
+      </c>
+      <c r="L5">
+        <v>0.978494623655914</v>
+      </c>
+      <c r="M5">
+        <v>0.96272401433691757</v>
+      </c>
+      <c r="N5">
+        <v>0.59211469534050176</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1120,34 +1222,19 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8">
-        <v>0.9173553719008265</v>
-      </c>
-      <c r="I8">
-        <v>0.60835629017447201</v>
-      </c>
-      <c r="J8">
-        <v>0.80991735537190079</v>
-      </c>
-      <c r="K8">
-        <v>0.86225895316804413</v>
-      </c>
-      <c r="L8">
-        <v>0.88705234159779611</v>
-      </c>
-      <c r="M8">
-        <v>0.87235996326905418</v>
-      </c>
-      <c r="N8">
-        <v>0.37741046831955921</v>
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9">
@@ -1157,6 +1244,15 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3"/>
@@ -1165,60 +1261,81 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>26</v>
+      </c>
+      <c r="O10" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="G11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11">
-        <v>0.99068100358422939</v>
-      </c>
-      <c r="I11">
-        <v>0.87813620071684584</v>
-      </c>
-      <c r="J11">
-        <v>0.95483870967741935</v>
-      </c>
-      <c r="K11">
-        <v>0.97347670250896057</v>
-      </c>
-      <c r="L11">
-        <v>0.978494623655914</v>
-      </c>
-      <c r="M11">
-        <v>0.96272401433691757</v>
-      </c>
-      <c r="N11">
-        <v>0.59211469534050176</v>
+        <v>29</v>
+      </c>
+      <c r="K11" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
+      <c r="G12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="3"/>
@@ -1227,6 +1344,12 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
+      <c r="K15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="3"/>
@@ -1239,7 +1362,7 @@
     <row r="17">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1247,15 +1370,15 @@
     <row r="18">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="G18" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -1265,30 +1388,30 @@
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="G19" s="5" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="H19" s="5"/>
       <c r="K19" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" ht="14.25">
       <c r="G20" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="K20" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" ht="15">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="G21" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="K21" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22">
@@ -1296,10 +1419,10 @@
         <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="K22" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23">
@@ -1307,10 +1430,10 @@
         <v>11</v>
       </c>
       <c r="G23" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="K23" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24">
@@ -1318,48 +1441,48 @@
         <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="K24" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="G25" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="K25" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="G26" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="K26" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" ht="14.25">
       <c r="G27" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="K27" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G28" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29">
@@ -1374,21 +1497,21 @@
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" ht="14.25"/>
     <row r="34">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="H34" s="5"/>
     </row>
@@ -1397,7 +1520,7 @@
         <v>11</v>
       </c>
       <c r="G35" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36">
@@ -1405,28 +1528,28 @@
         <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="G37" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="G38" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" ht="14.25">
       <c r="G39" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40">
@@ -1434,20 +1557,20 @@
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="G40" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" ht="14.25">
       <c r="G41" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" ht="15">
       <c r="A42" s="1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="G42" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43">
@@ -1455,7 +1578,7 @@
         <v>2</v>
       </c>
       <c r="G43" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44">
@@ -1470,17 +1593,17 @@
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50">
@@ -1488,7 +1611,7 @@
         <v>11</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
@@ -1498,36 +1621,36 @@
         <v>13</v>
       </c>
       <c r="G51" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="G52" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="G53" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" ht="14.25">
       <c r="G54" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="G55" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56">
@@ -1535,7 +1658,7 @@
         <v>11</v>
       </c>
       <c r="G56" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57">
@@ -1543,23 +1666,23 @@
         <v>13</v>
       </c>
       <c r="G57" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="G58" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="G59" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60" ht="14.25"/>
@@ -1571,38 +1694,38 @@
     <row r="62" ht="14.25"/>
     <row r="63" ht="15">
       <c r="A63" s="1" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" ht="14.25"/>
     <row r="70" ht="14.25">
       <c r="G70" s="5" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
@@ -1612,71 +1735,71 @@
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="G71" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" ht="14.25">
       <c r="G72" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" ht="15.75">
       <c r="A73" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="G73" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="G74" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="G75" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="G76" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="G77" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="G78" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" ht="14.25">
       <c r="G79" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" ht="14.25">
       <c r="J80" s="6"/>
       <c r="K80" s="5" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="L80" s="5"/>
     </row>
@@ -1685,51 +1808,51 @@
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="K81" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
     </row>
     <row r="82" ht="14.25">
       <c r="K82" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="83" ht="15.75">
       <c r="A83" s="1" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="K83" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
     </row>
     <row r="84">
       <c r="B84" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="C84" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="D84" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="E84" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="F84" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="G84" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="H84" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="K84" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
     </row>
     <row r="85">
       <c r="B85" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="C85">
         <v>118</v>
@@ -1750,12 +1873,12 @@
         <v>2</v>
       </c>
       <c r="K85" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
     </row>
     <row r="86">
       <c r="B86" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="C86">
         <v>14</v>
@@ -1776,12 +1899,12 @@
         <v>0</v>
       </c>
       <c r="K86" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="C87">
         <v>3</v>
@@ -1802,12 +1925,12 @@
         <v>1</v>
       </c>
       <c r="K87" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
     </row>
     <row r="88">
       <c r="B88" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -1828,12 +1951,12 @@
         <v>0</v>
       </c>
       <c r="K88" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -1854,12 +1977,12 @@
         <v>59</v>
       </c>
       <c r="K89" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
     </row>
     <row r="90">
       <c r="B90" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C90">
         <v>1</v>

</xml_diff>